<commit_message>
otazky -> vylepsenie vyhodnotenia
</commit_message>
<xml_diff>
--- a/app/src/main/assets/planety_quizz.xlsx
+++ b/app/src/main/assets/planety_quizz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/24b8b251d8fae0f4/PEVS/__BAKALARKA/app/src/main/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{C90CBB8E-5315-4C0C-B1B1-8548AA6FBBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E723306-D1DC-4BC7-BBE4-9A4457B025DC}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{C90CBB8E-5315-4C0C-B1B1-8548AA6FBBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12827E7D-0BE2-41E9-B279-5F5556CB84C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59B42603-5E37-44C8-B453-97DD41C0E15D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="127">
   <si>
     <t>SLNKO</t>
   </si>
@@ -177,6 +177,246 @@
   </si>
   <si>
     <t>URAN</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 1</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 2</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 3</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 4</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 5</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 6</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 7</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 8</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 9</t>
+  </si>
+  <si>
+    <t>Otazka Merkur 10</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 1</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 2</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 3</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 4</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 5</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 6</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 7</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 8</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 9</t>
+  </si>
+  <si>
+    <t>Otazka Venusa 10</t>
+  </si>
+  <si>
+    <t>Otazka Zem 1</t>
+  </si>
+  <si>
+    <t>Otazka Zem 2</t>
+  </si>
+  <si>
+    <t>Otazka Zem 3</t>
+  </si>
+  <si>
+    <t>Otazka Zem 4</t>
+  </si>
+  <si>
+    <t>Otazka Zem 5</t>
+  </si>
+  <si>
+    <t>Otazka Zem 6</t>
+  </si>
+  <si>
+    <t>Otazka Zem 7</t>
+  </si>
+  <si>
+    <t>Otazka Zem 8</t>
+  </si>
+  <si>
+    <t>Otazka Zem 9</t>
+  </si>
+  <si>
+    <t>Otazka Zem 10</t>
+  </si>
+  <si>
+    <t>Otazka mars 1</t>
+  </si>
+  <si>
+    <t>Otazka mars 2</t>
+  </si>
+  <si>
+    <t>Otazka mars 3</t>
+  </si>
+  <si>
+    <t>Otazka mars 4</t>
+  </si>
+  <si>
+    <t>Otazka mars 5</t>
+  </si>
+  <si>
+    <t>Otazka mars 6</t>
+  </si>
+  <si>
+    <t>Otazka mars 7</t>
+  </si>
+  <si>
+    <t>Otazka mars 8</t>
+  </si>
+  <si>
+    <t>Otazka mars 9</t>
+  </si>
+  <si>
+    <t>Otazka mars 10</t>
+  </si>
+  <si>
+    <t>otazka jupiter 1</t>
+  </si>
+  <si>
+    <t>otazka jupiter 2</t>
+  </si>
+  <si>
+    <t>otazka jupiter 3</t>
+  </si>
+  <si>
+    <t>otazka jupiter 4</t>
+  </si>
+  <si>
+    <t>otazka jupiter 5</t>
+  </si>
+  <si>
+    <t>otazka jupiter 6</t>
+  </si>
+  <si>
+    <t>otazka jupiter 7</t>
+  </si>
+  <si>
+    <t>otazka jupiter 8</t>
+  </si>
+  <si>
+    <t>otazka jupiter 9</t>
+  </si>
+  <si>
+    <t>otazka jupiter 10</t>
+  </si>
+  <si>
+    <t>Otazka saturn 1</t>
+  </si>
+  <si>
+    <t>Otazka saturn 2</t>
+  </si>
+  <si>
+    <t>Otazka saturn 3</t>
+  </si>
+  <si>
+    <t>Otazka saturn 4</t>
+  </si>
+  <si>
+    <t>Otazka saturn 5</t>
+  </si>
+  <si>
+    <t>Otazka saturn 6</t>
+  </si>
+  <si>
+    <t>Otazka saturn 7</t>
+  </si>
+  <si>
+    <t>Otazka saturn 8</t>
+  </si>
+  <si>
+    <t>Otazka saturn 9</t>
+  </si>
+  <si>
+    <t>Otazka saturn 10</t>
+  </si>
+  <si>
+    <t>Otazka uran 1</t>
+  </si>
+  <si>
+    <t>Otazka uran 2</t>
+  </si>
+  <si>
+    <t>Otazka uran 3</t>
+  </si>
+  <si>
+    <t>Otazka uran 4</t>
+  </si>
+  <si>
+    <t>Otazka uran 5</t>
+  </si>
+  <si>
+    <t>Otazka uran 6</t>
+  </si>
+  <si>
+    <t>Otazka uran 7</t>
+  </si>
+  <si>
+    <t>Otazka uran 8</t>
+  </si>
+  <si>
+    <t>Otazka uran 9</t>
+  </si>
+  <si>
+    <t>Otazka uran 10</t>
+  </si>
+  <si>
+    <t>Otazka neptun 1</t>
+  </si>
+  <si>
+    <t>Otazka neptun 2</t>
+  </si>
+  <si>
+    <t>Otazka neptun 3</t>
+  </si>
+  <si>
+    <t>Otazka neptun 4</t>
+  </si>
+  <si>
+    <t>Otazka neptun 5</t>
+  </si>
+  <si>
+    <t>Otazka neptun 6</t>
+  </si>
+  <si>
+    <t>Otazka neptun 7</t>
+  </si>
+  <si>
+    <t>Otazka neptun 8</t>
+  </si>
+  <si>
+    <t>Otazka neptun 9</t>
+  </si>
+  <si>
+    <t>Otazka neptun 10</t>
   </si>
 </sst>
 </file>
@@ -542,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EE18A4-0E79-4F3E-B37F-340BDF55F156}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -726,7 +966,7 @@
         <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -743,7 +983,7 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -760,7 +1000,7 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -777,7 +1017,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -794,7 +1034,7 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -811,7 +1051,7 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -828,7 +1068,7 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -845,7 +1085,7 @@
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -862,7 +1102,7 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
@@ -879,7 +1119,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
@@ -896,7 +1136,7 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -913,7 +1153,7 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -930,7 +1170,7 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -947,7 +1187,7 @@
         <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -964,7 +1204,7 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -981,7 +1221,7 @@
         <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -998,7 +1238,7 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1015,7 +1255,7 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -1032,7 +1272,7 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -1049,7 +1289,7 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -1066,7 +1306,7 @@
         <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -1083,7 +1323,7 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1100,7 +1340,7 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -1117,7 +1357,7 @@
         <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1134,7 +1374,7 @@
         <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
@@ -1151,7 +1391,7 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1168,7 +1408,7 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -1185,7 +1425,7 @@
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
@@ -1202,7 +1442,7 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
@@ -1219,7 +1459,7 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
@@ -1236,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1253,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1270,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -1287,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1304,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
@@ -1321,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -1338,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
@@ -1355,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
@@ -1372,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
@@ -1389,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
@@ -1406,7 +1646,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -1423,7 +1663,7 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1440,7 +1680,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -1457,7 +1697,7 @@
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
@@ -1474,7 +1714,7 @@
         <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
@@ -1491,7 +1731,7 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
         <v>11</v>
@@ -1508,7 +1748,7 @@
         <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
@@ -1525,7 +1765,7 @@
         <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C58" t="s">
         <v>13</v>
@@ -1542,7 +1782,7 @@
         <v>43</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="C59" t="s">
         <v>14</v>
@@ -1559,7 +1799,7 @@
         <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
@@ -1576,7 +1816,7 @@
         <v>44</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1593,7 +1833,7 @@
         <v>44</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -1610,7 +1850,7 @@
         <v>44</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -1627,7 +1867,7 @@
         <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -1644,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C65" t="s">
         <v>10</v>
@@ -1661,7 +1901,7 @@
         <v>44</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -1678,7 +1918,7 @@
         <v>44</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -1695,7 +1935,7 @@
         <v>44</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="C68" t="s">
         <v>13</v>
@@ -1712,7 +1952,7 @@
         <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="C69" t="s">
         <v>14</v>
@@ -1729,7 +1969,7 @@
         <v>44</v>
       </c>
       <c r="B70" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
         <v>15</v>
@@ -1746,7 +1986,7 @@
         <v>46</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
@@ -1763,7 +2003,7 @@
         <v>46</v>
       </c>
       <c r="B72" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C72" t="s">
         <v>7</v>
@@ -1780,7 +2020,7 @@
         <v>46</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -1797,7 +2037,7 @@
         <v>46</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -1814,7 +2054,7 @@
         <v>46</v>
       </c>
       <c r="B75" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="C75" t="s">
         <v>10</v>
@@ -1831,7 +2071,7 @@
         <v>46</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -1848,7 +2088,7 @@
         <v>46</v>
       </c>
       <c r="B77" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
@@ -1865,7 +2105,7 @@
         <v>46</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
@@ -1882,7 +2122,7 @@
         <v>46</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C79" t="s">
         <v>14</v>
@@ -1899,7 +2139,7 @@
         <v>46</v>
       </c>
       <c r="B80" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
@@ -1916,7 +2156,7 @@
         <v>45</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
@@ -1933,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
@@ -1950,7 +2190,7 @@
         <v>45</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="C83" t="s">
         <v>8</v>
@@ -1967,7 +2207,7 @@
         <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
@@ -1984,7 +2224,7 @@
         <v>45</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C85" t="s">
         <v>10</v>
@@ -2001,7 +2241,7 @@
         <v>45</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="C86" t="s">
         <v>11</v>
@@ -2018,7 +2258,7 @@
         <v>45</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="C87" t="s">
         <v>12</v>
@@ -2035,7 +2275,7 @@
         <v>45</v>
       </c>
       <c r="B88" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="C88" t="s">
         <v>13</v>
@@ -2052,7 +2292,7 @@
         <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="C89" t="s">
         <v>14</v>
@@ -2069,7 +2309,7 @@
         <v>45</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="C90" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
implementacia Toda a zacatie doplnanie planet
</commit_message>
<xml_diff>
--- a/app/src/main/assets/planety_quizz.xlsx
+++ b/app/src/main/assets/planety_quizz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/24b8b251d8fae0f4/PEVS/__BAKALARKA/app/src/main/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{C90CBB8E-5315-4C0C-B1B1-8548AA6FBBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EB76317-C1D5-4B12-A1BD-CE2D843A2219}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{C90CBB8E-5315-4C0C-B1B1-8548AA6FBBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36477707-8F7D-4918-859C-8C47AF6CD906}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59B42603-5E37-44C8-B453-97DD41C0E15D}"/>
+    <workbookView xWindow="4776" yWindow="6408" windowWidth="17280" windowHeight="8880" xr2:uid="{59B42603-5E37-44C8-B453-97DD41C0E15D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="165">
   <si>
     <t>SLNKO</t>
   </si>
@@ -149,36 +149,6 @@
     <t>URAN</t>
   </si>
   <si>
-    <t>Otazka Merkur 1</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 2</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 3</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 4</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 5</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 6</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 7</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 8</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 9</t>
-  </si>
-  <si>
-    <t>Otazka Merkur 10</t>
-  </si>
-  <si>
     <t>Otazka Venusa 1</t>
   </si>
   <si>
@@ -461,28 +431,106 @@
     <t>Iba pre mimozenštanov</t>
   </si>
   <si>
-    <t>Aké ťažké je Slnko?</t>
-  </si>
-  <si>
-    <t>Tvorí 99,87% slnečnej sústavy</t>
-  </si>
-  <si>
-    <t>Čo robí gravitačné pole Slnka?</t>
-  </si>
-  <si>
-    <t>Udržuje všetky planéty na obežných dráhach</t>
-  </si>
-  <si>
-    <t>Také ťažké ako tvoj otec</t>
-  </si>
-  <si>
-    <t>O niečo ťažšíe ako slon</t>
-  </si>
-  <si>
-    <t>Udržuje vtáky vo vzduchu</t>
-  </si>
-  <si>
-    <t>Vďaka nemu lietajú vesmírne lode</t>
+    <t>Aká je najvrchnejšia časť Slnka?</t>
+  </si>
+  <si>
+    <t>Koróna</t>
+  </si>
+  <si>
+    <t>Fotosféra</t>
+  </si>
+  <si>
+    <t>Niečo žlté</t>
+  </si>
+  <si>
+    <t>Čo sú slnečné škvrny?</t>
+  </si>
+  <si>
+    <t>Chladnejšie časti Slnka</t>
+  </si>
+  <si>
+    <t>Slnko sa neumylo</t>
+  </si>
+  <si>
+    <t>Niekto tam nechal plachtu</t>
+  </si>
+  <si>
+    <t>Kde sa nachádza Merkúr?</t>
+  </si>
+  <si>
+    <t>Najbližšie ku Slnku</t>
+  </si>
+  <si>
+    <t>Najďalej pri Slnku</t>
+  </si>
+  <si>
+    <t>V n124qw galaxií</t>
+  </si>
+  <si>
+    <t>Aká je veľkosť Merkúru</t>
+  </si>
+  <si>
+    <t>Patrí medzi druhú najmenšiu</t>
+  </si>
+  <si>
+    <t>Je najväčšia</t>
+  </si>
+  <si>
+    <t>Skoro rovnaká ako Zem</t>
+  </si>
+  <si>
+    <t>Má nejakú atmosféru?</t>
+  </si>
+  <si>
+    <t>Takmer žiadnu</t>
+  </si>
+  <si>
+    <t>Čo je armosféra?</t>
+  </si>
+  <si>
+    <t>Aké sú najväčšie teploty?</t>
+  </si>
+  <si>
+    <t>430 C</t>
+  </si>
+  <si>
+    <t>1500 C</t>
+  </si>
+  <si>
+    <t>589 C</t>
+  </si>
+  <si>
+    <t>Aká je najnižšia teplota?</t>
+  </si>
+  <si>
+    <t>Čím je pokrytý Merkúr?</t>
+  </si>
+  <si>
+    <t>Koľko mesiacov má Merkúr?</t>
+  </si>
+  <si>
+    <t>Koľko trvá dĺžka roka  na Merkúre?</t>
+  </si>
+  <si>
+    <t>Prečo nemá takmer žiadnu atmosféru?</t>
+  </si>
+  <si>
+    <t>Hmotnosť planéty je príliš malá</t>
+  </si>
+  <si>
+    <t>Atmosféra nemá rada Merkúr</t>
+  </si>
+  <si>
+    <t>Čo je to atmosféra?</t>
+  </si>
+  <si>
+    <t>Koľko ročných období má Merkúr?</t>
+  </si>
+  <si>
+    <t>Žiadne</t>
+  </si>
+  <si>
+    <t>Jar a Leto</t>
   </si>
 </sst>
 </file>
@@ -848,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EE18A4-0E79-4F3E-B37F-340BDF55F156}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,16 +910,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,16 +927,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -896,16 +944,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -913,16 +961,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -930,16 +978,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -947,16 +995,16 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -964,16 +1012,16 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -981,16 +1029,16 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -998,16 +1046,16 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1015,16 +1063,16 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,16 +1080,16 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,16 +1097,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1066,16 +1114,16 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
+        <v>154</v>
+      </c>
+      <c r="C13">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>-180</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1083,7 +1131,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1100,16 +1148,16 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
+        <v>156</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,16 +1165,16 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
+        <v>157</v>
+      </c>
+      <c r="C16">
+        <v>66</v>
+      </c>
+      <c r="D16">
+        <v>77</v>
+      </c>
+      <c r="E16">
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1134,16 +1182,16 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1151,16 +1199,16 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
+        <v>162</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1168,7 +1216,7 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1185,7 +1233,7 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -1202,7 +1250,7 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1219,7 +1267,7 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1236,7 +1284,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -1253,7 +1301,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -1270,7 +1318,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -1287,7 +1335,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1304,7 +1352,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -1321,7 +1369,7 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -1338,7 +1386,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1355,7 +1403,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -1372,7 +1420,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1389,7 +1437,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1406,7 +1454,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -1423,7 +1471,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1440,7 +1488,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -1457,7 +1505,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -1474,7 +1522,7 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
@@ -1491,7 +1539,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -1508,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -1525,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -1542,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1559,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1576,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1593,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1610,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -1627,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1644,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -1661,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -1678,7 +1726,7 @@
         <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -1695,7 +1743,7 @@
         <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -1712,7 +1760,7 @@
         <v>33</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -1729,7 +1777,7 @@
         <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1746,7 +1794,7 @@
         <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -1763,7 +1811,7 @@
         <v>33</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -1780,7 +1828,7 @@
         <v>33</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -1797,7 +1845,7 @@
         <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -1814,7 +1862,7 @@
         <v>33</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
         <v>10</v>
@@ -1831,7 +1879,7 @@
         <v>33</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
@@ -1848,7 +1896,7 @@
         <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -1865,7 +1913,7 @@
         <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
@@ -1882,7 +1930,7 @@
         <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -1899,7 +1947,7 @@
         <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1916,7 +1964,7 @@
         <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
@@ -1933,7 +1981,7 @@
         <v>34</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
@@ -1950,7 +1998,7 @@
         <v>34</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
@@ -1967,7 +2015,7 @@
         <v>34</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -1984,7 +2032,7 @@
         <v>34</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
         <v>10</v>
@@ -2001,7 +2049,7 @@
         <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
         <v>11</v>
@@ -2018,7 +2066,7 @@
         <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -2035,7 +2083,7 @@
         <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
@@ -2052,7 +2100,7 @@
         <v>36</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -2069,7 +2117,7 @@
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2086,7 +2134,7 @@
         <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
@@ -2103,7 +2151,7 @@
         <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C74" t="s">
         <v>7</v>
@@ -2120,7 +2168,7 @@
         <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
@@ -2137,7 +2185,7 @@
         <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
@@ -2154,7 +2202,7 @@
         <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
         <v>10</v>
@@ -2171,7 +2219,7 @@
         <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C78" t="s">
         <v>11</v>
@@ -2188,7 +2236,7 @@
         <v>35</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C79" t="s">
         <v>2</v>
@@ -2205,7 +2253,7 @@
         <v>35</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
@@ -2222,7 +2270,7 @@
         <v>35</v>
       </c>
       <c r="B81" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -2239,7 +2287,7 @@
         <v>35</v>
       </c>
       <c r="B82" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2256,7 +2304,7 @@
         <v>35</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
@@ -2273,7 +2321,7 @@
         <v>35</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -2290,7 +2338,7 @@
         <v>35</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -2307,7 +2355,7 @@
         <v>35</v>
       </c>
       <c r="B86" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
@@ -2324,7 +2372,7 @@
         <v>35</v>
       </c>
       <c r="B87" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
@@ -2341,7 +2389,7 @@
         <v>35</v>
       </c>
       <c r="B88" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C88" t="s">
         <v>11</v>

</xml_diff>